<commit_message>
Mejor manejo de los materiales
</commit_message>
<xml_diff>
--- a/Presupuesto TAG.xlsx
+++ b/Presupuesto TAG.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tecnico\Work\tag2\TAG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shize\TAG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4CBDE6-C35D-4D17-895D-C3FB6B9E449C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1388018E-6ECD-4AB4-A1EC-715CE0DD4835}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principal - ABP" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="247">
   <si>
     <t>Apellidos</t>
   </si>
@@ -1134,9 +1134,6 @@
     <t>David la creación y Javi el manejo</t>
   </si>
   <si>
-    <t>David shader con materiales y Javi el sombreado</t>
-  </si>
-  <si>
     <t>David creó la base de la fachada, Javi creó el árbol, y después ciclos de implementaciones de Javi y reorganización de David. Es 50% porque actualmente es el 100% del código pero faltan cosas</t>
   </si>
   <si>
@@ -1144,6 +1141,24 @@
   </si>
   <si>
     <t>Falta asegurar la integración con el proyecto</t>
+  </si>
+  <si>
+    <t>Falta probar en vivo la gestión de materiales</t>
+  </si>
+  <si>
+    <t>Falta de Shader con Phong</t>
+  </si>
+  <si>
+    <t>David shader con materiales y Javi el sombreado sin Phong</t>
+  </si>
+  <si>
+    <t>La lectura es correcta, pero no cubre todas las declaraciones del fichero .mtl</t>
+  </si>
+  <si>
+    <t>Hipotesis</t>
+  </si>
+  <si>
+    <t>Progreso</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1167,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="0.00;[Red]\-0.00;&quot;&quot;"/>
-    <numFmt numFmtId="168" formatCode="0\ %"/>
+    <numFmt numFmtId="165" formatCode="0.00;[Red]\-0.00;&quot;&quot;"/>
+    <numFmt numFmtId="166" formatCode="0\ %"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1464,7 +1479,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1848,6 +1863,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2008,9 +2036,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2102,7 +2130,7 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="145" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="16" borderId="1" xfId="145" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="23" fillId="16" borderId="1" xfId="145" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2125,7 +2153,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="16" borderId="12" xfId="145" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="165" fontId="23" fillId="16" borderId="12" xfId="145" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="21" fillId="15" borderId="12" xfId="145" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -2173,6 +2201,11 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="145" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="145" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="145" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2235,9 +2268,27 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="12" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="25" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2247,26 +2298,37 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="145" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="12" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="145" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="145" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="145" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="145" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="145" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="12" borderId="0" xfId="145" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="145" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="11" borderId="31" xfId="145" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="16" borderId="13" xfId="145" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="1" xfId="145" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="145" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="145" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="145" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="159">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8" hidden="1"/>
@@ -2806,113 +2868,113 @@
   <sheetData>
     <row r="1" spans="2:18" ht="16.5" thickBot="1"/>
     <row r="2" spans="2:18" ht="23.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="79" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="78"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="81"/>
     </row>
     <row r="3" spans="2:18" ht="46.9" customHeight="1">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="81"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="84"/>
     </row>
     <row r="4" spans="2:18">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="87"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="90"/>
     </row>
     <row r="5" spans="2:18">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="90"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="92"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="93"/>
     </row>
     <row r="6" spans="2:18" ht="16.5" thickBot="1">
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="84"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="86"/>
+      <c r="R6" s="87"/>
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="2"/>
@@ -2956,30 +3018,30 @@
       <c r="B9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="91"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="92"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="95"/>
     </row>
     <row r="11" spans="2:18">
-      <c r="E11" s="73" t="s">
+      <c r="E11" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="73"/>
-      <c r="G11" s="74" t="s">
+      <c r="F11" s="76"/>
+      <c r="G11" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="75" t="s">
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="75"/>
-      <c r="P11" s="75"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
+      <c r="O11" s="78"/>
+      <c r="P11" s="78"/>
     </row>
     <row r="12" spans="2:18" s="8" customFormat="1" ht="79.5" thickBot="1">
       <c r="B12" s="3" t="s">
@@ -3356,10 +3418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="E54" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="12.75"/>
@@ -3370,43 +3432,47 @@
     <col min="4" max="4" width="107.125" style="23" customWidth="1"/>
     <col min="5" max="8" width="8.75" style="23"/>
     <col min="9" max="9" width="9.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.25" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="144.875" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.75" style="23"/>
+    <col min="10" max="10" width="7.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.25" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="144.875" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.75" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.25">
-      <c r="A1" s="94" t="s">
+    <row r="1" spans="1:14" ht="23.25">
+      <c r="A1" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-    </row>
-    <row r="2" spans="1:13" ht="190.15" customHeight="1" thickBot="1">
-      <c r="A2" s="95" t="s">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="106"/>
+    </row>
+    <row r="2" spans="1:14" ht="190.15" customHeight="1" thickBot="1">
+      <c r="A2" s="104" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="107"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="24"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -3418,25 +3484,27 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
-    </row>
-    <row r="4" spans="1:13" ht="20.65" customHeight="1">
-      <c r="A4" s="96" t="s">
+      <c r="L3" s="24"/>
+    </row>
+    <row r="4" spans="1:14" ht="20.65" customHeight="1">
+      <c r="A4" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="96"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="38"/>
       <c r="D4" s="24"/>
-      <c r="E4" s="96" t="s">
+      <c r="E4" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75">
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="73"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75">
       <c r="A5" s="25" t="s">
         <v>33</v>
       </c>
@@ -3445,20 +3513,21 @@
       </c>
       <c r="C5" s="65"/>
       <c r="D5" s="24"/>
-      <c r="E5" s="93" t="s">
+      <c r="E5" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
       <c r="K5" s="27">
         <f>'Principal - ABP'!F19</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75">
+      <c r="L5" s="108"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75">
       <c r="A6" s="28" t="s">
         <v>36</v>
       </c>
@@ -3467,20 +3536,21 @@
       </c>
       <c r="C6" s="64"/>
       <c r="D6" s="24"/>
-      <c r="E6" s="93" t="s">
+      <c r="E6" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
       <c r="K6" s="29">
         <f>K5*B7</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75">
+      <c r="L6" s="109"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75">
       <c r="A7" s="28" t="s">
         <v>38</v>
       </c>
@@ -3489,38 +3559,40 @@
       </c>
       <c r="C7" s="64"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="93" t="s">
+      <c r="E7" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
       <c r="K7" s="30">
         <f>H13</f>
         <v>325</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="20.25" customHeight="1">
+      <c r="L7" s="110"/>
+    </row>
+    <row r="8" spans="1:14" ht="20.25" customHeight="1">
       <c r="A8" s="28"/>
       <c r="B8" s="27"/>
       <c r="C8" s="64"/>
       <c r="D8" s="24"/>
-      <c r="E8" s="93" t="s">
+      <c r="E8" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
       <c r="K8" s="31">
         <f>ABS(K6-K7)/K6</f>
         <v>0.35416666666666669</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="18.75">
+      <c r="L8" s="111"/>
+    </row>
+    <row r="9" spans="1:14" ht="18.75">
       <c r="A9" s="32" t="s">
         <v>29</v>
       </c>
@@ -3542,8 +3614,9 @@
         <f>I13</f>
         <v>27.083333333333332</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="L9" s="112"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="24"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
@@ -3555,15 +3628,16 @@
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
       <c r="K10" s="24"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1">
+      <c r="L10" s="24"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1">
       <c r="A11" s="100" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="100" t="s">
         <v>190</v>
       </c>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="96" t="s">
         <v>189</v>
       </c>
       <c r="D11" s="100" t="s">
@@ -3583,10 +3657,10 @@
       </c>
       <c r="I11" s="102"/>
     </row>
-    <row r="12" spans="1:13" ht="14.25">
+    <row r="12" spans="1:14" ht="14.25">
       <c r="A12" s="100"/>
       <c r="B12" s="100"/>
-      <c r="C12" s="98"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="100"/>
       <c r="E12" s="101"/>
       <c r="F12" s="101"/>
@@ -3599,8 +3673,12 @@
       <c r="I12" s="36" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="18.75">
+      <c r="K12" s="113" t="s">
+        <v>245</v>
+      </c>
+      <c r="L12" s="113"/>
+    </row>
+    <row r="13" spans="1:14" ht="18.75">
       <c r="A13" s="61"/>
       <c r="B13" s="60"/>
       <c r="C13" s="60"/>
@@ -3612,18 +3690,27 @@
         <f>SUM(H14:H82)</f>
         <v>325</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="114">
         <f>SUM(I14:I82)</f>
         <v>27.083333333333332</v>
       </c>
+      <c r="J13" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>47</v>
+      </c>
       <c r="L13" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="M13" s="23" t="s">
+      <c r="N13" s="23" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75">
+    <row r="14" spans="1:14" ht="15.75">
       <c r="A14" s="44" t="s">
         <v>188</v>
       </c>
@@ -3650,18 +3737,22 @@
         <f t="shared" ref="I14:I45" si="0">H14/$K$6*10*$K$5</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="J14" s="104">
+      <c r="J14" s="116">
         <v>1</v>
       </c>
-      <c r="K14" s="103">
+      <c r="K14" s="117">
         <f>I14*J14</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="L14" s="23" t="s">
+      <c r="L14" s="117">
+        <f>H14*J14</f>
+        <v>7</v>
+      </c>
+      <c r="M14" s="118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75">
+    <row r="15" spans="1:14" ht="15.75">
       <c r="A15" s="44" t="s">
         <v>186</v>
       </c>
@@ -3688,18 +3779,22 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="J15" s="104">
+      <c r="J15" s="116">
         <v>1</v>
       </c>
-      <c r="K15" s="103">
-        <f t="shared" ref="K15:L65" si="1">I15*J15</f>
+      <c r="K15" s="117">
+        <f t="shared" ref="K15:K65" si="1">I15*J15</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="117">
+        <f t="shared" ref="L15:L78" si="2">H15*J15</f>
+        <v>7</v>
+      </c>
+      <c r="M15" s="118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75">
+    <row r="16" spans="1:14" ht="15.75">
       <c r="A16" s="44" t="s">
         <v>184</v>
       </c>
@@ -3720,14 +3815,15 @@
         <v>49</v>
       </c>
       <c r="H16" s="47"/>
-      <c r="I16" s="39">
+      <c r="I16" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="104"/>
-      <c r="K16" s="103"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.75">
+      <c r="J16" s="75"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75">
       <c r="A17" s="44" t="s">
         <v>182</v>
       </c>
@@ -3754,18 +3850,22 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="J17" s="104">
+      <c r="J17" s="116">
         <v>1</v>
       </c>
-      <c r="K17" s="103">
+      <c r="K17" s="117">
         <f t="shared" si="1"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="L17" s="23" t="s">
+      <c r="L17" s="117">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="M17" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75">
+    <row r="18" spans="1:14" ht="15.75">
       <c r="A18" s="44" t="s">
         <v>180</v>
       </c>
@@ -3792,21 +3892,25 @@
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J18" s="104">
+      <c r="J18" s="116">
         <v>1</v>
       </c>
-      <c r="K18" s="103">
+      <c r="K18" s="117">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="117">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M18" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="M18" s="23" t="s">
+      <c r="N18" s="23" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75">
+    <row r="19" spans="1:14" ht="15.75">
       <c r="A19" s="44" t="s">
         <v>177</v>
       </c>
@@ -3833,18 +3937,22 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="J19" s="104">
+      <c r="J19" s="116">
         <v>1</v>
       </c>
-      <c r="K19" s="103">
+      <c r="K19" s="117">
         <f t="shared" si="1"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="117">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="M19" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75">
+    <row r="20" spans="1:14" ht="15.75">
       <c r="A20" s="44" t="s">
         <v>175</v>
       </c>
@@ -3871,21 +3979,25 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="J20" s="104">
+      <c r="J20" s="116">
         <v>1</v>
       </c>
-      <c r="K20" s="103">
+      <c r="K20" s="117">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L20" s="23" t="s">
+      <c r="L20" s="117">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M20" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="M20" s="23" t="s">
+      <c r="N20" s="23" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75">
+    <row r="21" spans="1:14" ht="15.75">
       <c r="A21" s="44" t="s">
         <v>174</v>
       </c>
@@ -3912,21 +4024,25 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="J21" s="104">
+      <c r="J21" s="116">
         <v>1</v>
       </c>
-      <c r="K21" s="103">
+      <c r="K21" s="117">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L21" s="23" t="s">
+      <c r="L21" s="117">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M21" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="M21" s="23" t="s">
+      <c r="N21" s="23" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75">
+    <row r="22" spans="1:14" ht="15.75">
       <c r="A22" s="44" t="s">
         <v>172</v>
       </c>
@@ -3953,18 +4069,22 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J22" s="104">
+      <c r="J22" s="116">
         <v>1</v>
       </c>
-      <c r="K22" s="103">
+      <c r="K22" s="117">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="L22" s="23" t="s">
+      <c r="L22" s="117">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M22" s="118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75">
+    <row r="23" spans="1:14" ht="15.75">
       <c r="A23" s="44" t="s">
         <v>170</v>
       </c>
@@ -3991,18 +4111,22 @@
         <f t="shared" si="0"/>
         <v>0.41666666666666663</v>
       </c>
-      <c r="J23" s="104">
+      <c r="J23" s="116">
         <v>1</v>
       </c>
-      <c r="K23" s="103">
+      <c r="K23" s="117">
         <f t="shared" si="1"/>
         <v>0.41666666666666663</v>
       </c>
-      <c r="L23" s="23" t="s">
+      <c r="L23" s="117">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="M23" s="118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75">
+    <row r="24" spans="1:14" ht="15.75">
       <c r="A24" s="44" t="s">
         <v>169</v>
       </c>
@@ -4029,18 +4153,22 @@
         <f t="shared" si="0"/>
         <v>0.41666666666666663</v>
       </c>
-      <c r="J24" s="104">
+      <c r="J24" s="116">
         <v>1</v>
       </c>
-      <c r="K24" s="103">
+      <c r="K24" s="117">
         <f t="shared" si="1"/>
         <v>0.41666666666666663</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="117">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="M24" s="118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75">
+    <row r="25" spans="1:14" ht="15.75">
       <c r="A25" s="44" t="s">
         <v>168</v>
       </c>
@@ -4065,10 +4193,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J25" s="104"/>
-      <c r="K25" s="103"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75">
+      <c r="J25" s="75"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="74"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75">
       <c r="A26" s="44" t="s">
         <v>165</v>
       </c>
@@ -4095,18 +4224,22 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J26" s="104">
+      <c r="J26" s="116">
         <v>1</v>
       </c>
-      <c r="K26" s="103">
+      <c r="K26" s="117">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="L26" s="23" t="s">
+      <c r="L26" s="117">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M26" s="118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75">
+    <row r="27" spans="1:14" ht="15.75">
       <c r="A27" s="44" t="s">
         <v>163</v>
       </c>
@@ -4133,18 +4266,22 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J27" s="104">
+      <c r="J27" s="116">
         <v>1</v>
       </c>
-      <c r="K27" s="103">
+      <c r="K27" s="117">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="L27" s="23" t="s">
+      <c r="L27" s="117">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M27" s="118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75">
+    <row r="28" spans="1:14" ht="15.75">
       <c r="A28" s="44" t="s">
         <v>161</v>
       </c>
@@ -4169,10 +4306,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J28" s="104"/>
-      <c r="K28" s="103"/>
-    </row>
-    <row r="29" spans="1:13" ht="15.75">
+      <c r="J28" s="75"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="74"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75">
       <c r="A29" s="44" t="s">
         <v>159</v>
       </c>
@@ -4197,10 +4335,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="104"/>
-      <c r="K29" s="103"/>
-    </row>
-    <row r="30" spans="1:13" ht="15.75">
+      <c r="J29" s="75"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="74"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75">
       <c r="A30" s="44" t="s">
         <v>156</v>
       </c>
@@ -4227,18 +4366,22 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J30" s="104">
+      <c r="J30" s="116">
         <v>1</v>
       </c>
-      <c r="K30" s="103">
+      <c r="K30" s="117">
         <f>I30*J30</f>
         <v>0.5</v>
       </c>
-      <c r="L30" s="23" t="s">
+      <c r="L30" s="117">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M30" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75">
+    <row r="31" spans="1:14" ht="15.75">
       <c r="A31" s="44" t="s">
         <v>154</v>
       </c>
@@ -4265,21 +4408,25 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="J31" s="104">
-        <v>0.66</v>
-      </c>
-      <c r="K31" s="103">
+      <c r="J31" s="116">
+        <v>0.9</v>
+      </c>
+      <c r="K31" s="117">
         <f t="shared" si="1"/>
-        <v>0.38500000000000006</v>
-      </c>
-      <c r="L31" s="23" t="s">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="L31" s="117">
+        <f t="shared" si="2"/>
+        <v>6.3</v>
+      </c>
+      <c r="M31" s="118" t="s">
         <v>222</v>
       </c>
-      <c r="M31" s="23" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.75">
+      <c r="N31" s="23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75">
       <c r="A32" s="44" t="s">
         <v>152</v>
       </c>
@@ -4306,21 +4453,25 @@
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J32" s="104">
+      <c r="J32" s="116">
         <v>0.75</v>
       </c>
-      <c r="K32" s="103">
+      <c r="K32" s="117">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="L32" s="23" t="s">
+      <c r="L32" s="117">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M32" s="118" t="s">
         <v>222</v>
       </c>
-      <c r="M32" s="23" t="s">
+      <c r="N32" s="23" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75">
+    <row r="33" spans="1:14" ht="15.75">
       <c r="A33" s="44" t="s">
         <v>150</v>
       </c>
@@ -4345,10 +4496,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J33" s="104"/>
-      <c r="K33" s="103"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.75">
+      <c r="J33" s="75"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.75">
       <c r="A34" s="44" t="s">
         <v>148</v>
       </c>
@@ -4373,10 +4525,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J34" s="104"/>
-      <c r="K34" s="103"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.75">
+      <c r="J34" s="75"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="74"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75">
       <c r="A35" s="44" t="s">
         <v>146</v>
       </c>
@@ -4401,10 +4554,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J35" s="104"/>
-      <c r="K35" s="103"/>
-    </row>
-    <row r="36" spans="1:12" ht="15.75">
+      <c r="J35" s="75"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75">
       <c r="A36" s="44" t="s">
         <v>145</v>
       </c>
@@ -4429,10 +4583,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J36" s="104"/>
-      <c r="K36" s="103"/>
-    </row>
-    <row r="37" spans="1:12" ht="15.75">
+      <c r="J36" s="75"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="74"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75">
       <c r="A37" s="44" t="s">
         <v>142</v>
       </c>
@@ -4459,18 +4614,25 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="J37" s="104">
-        <v>0.75</v>
-      </c>
-      <c r="K37" s="103">
+      <c r="J37" s="116">
+        <v>0.9</v>
+      </c>
+      <c r="K37" s="117">
         <f t="shared" si="1"/>
-        <v>0.4375</v>
-      </c>
-      <c r="L37" s="23" t="s">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="L37" s="117">
+        <f t="shared" si="2"/>
+        <v>6.3</v>
+      </c>
+      <c r="M37" s="118" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="15.75">
+      <c r="N37" s="23" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15.75">
       <c r="A38" s="44" t="s">
         <v>140</v>
       </c>
@@ -4497,18 +4659,22 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="J38" s="104">
+      <c r="J38" s="116">
         <v>1</v>
       </c>
-      <c r="K38" s="103">
+      <c r="K38" s="117">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L38" s="103" t="s">
+      <c r="L38" s="117">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M38" s="117" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75">
+    <row r="39" spans="1:14" ht="15.75">
       <c r="A39" s="44" t="s">
         <v>138</v>
       </c>
@@ -4535,18 +4701,22 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J39" s="104">
+      <c r="J39" s="116">
         <v>1</v>
       </c>
-      <c r="K39" s="103">
+      <c r="K39" s="117">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="L39" s="23" t="s">
+      <c r="L39" s="117">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M39" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75">
+    <row r="40" spans="1:14" ht="15.75">
       <c r="A40" s="44" t="s">
         <v>135</v>
       </c>
@@ -4573,18 +4743,22 @@
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="J40" s="104">
+      <c r="J40" s="116">
         <v>1</v>
       </c>
-      <c r="K40" s="103">
+      <c r="K40" s="117">
         <f t="shared" si="1"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="L40" s="23" t="s">
+      <c r="L40" s="117">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="M40" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75">
+    <row r="41" spans="1:14" ht="15.75">
       <c r="A41" s="44" t="s">
         <v>133</v>
       </c>
@@ -4611,18 +4785,22 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="J41" s="104">
+      <c r="J41" s="116">
         <v>1</v>
       </c>
-      <c r="K41" s="103">
+      <c r="K41" s="117">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L41" s="23" t="s">
+      <c r="L41" s="117">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M41" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75">
+    <row r="42" spans="1:14" ht="15.75">
       <c r="A42" s="44" t="s">
         <v>131</v>
       </c>
@@ -4649,18 +4827,22 @@
         <f t="shared" si="0"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="J42" s="104">
+      <c r="J42" s="116">
         <v>1</v>
       </c>
-      <c r="K42" s="103">
+      <c r="K42" s="117">
         <f t="shared" si="1"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="L42" s="23" t="s">
+      <c r="L42" s="117">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="M42" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75">
+    <row r="43" spans="1:14" ht="15.75">
       <c r="A43" s="44" t="s">
         <v>129</v>
       </c>
@@ -4687,18 +4869,22 @@
         <f t="shared" si="0"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="J43" s="104">
+      <c r="J43" s="116">
         <v>1</v>
       </c>
-      <c r="K43" s="103">
+      <c r="K43" s="117">
         <f t="shared" si="1"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="L43" s="23" t="s">
+      <c r="L43" s="117">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="M43" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75">
+    <row r="44" spans="1:14" ht="15.75">
       <c r="A44" s="44" t="s">
         <v>127</v>
       </c>
@@ -4723,10 +4909,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J44" s="104"/>
-      <c r="K44" s="103"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.75">
+      <c r="J44" s="75"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="74"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75">
       <c r="A45" s="44" t="s">
         <v>125</v>
       </c>
@@ -4751,10 +4938,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J45" s="104"/>
-      <c r="K45" s="103"/>
-    </row>
-    <row r="46" spans="1:12" ht="15.75">
+      <c r="J45" s="75"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="74"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.75">
       <c r="A46" s="44" t="s">
         <v>124</v>
       </c>
@@ -4776,13 +4964,14 @@
       </c>
       <c r="H46" s="47"/>
       <c r="I46" s="39">
-        <f t="shared" ref="I46:I77" si="2">H46/$K$6*10*$K$5</f>
-        <v>0</v>
-      </c>
-      <c r="J46" s="104"/>
-      <c r="K46" s="103"/>
-    </row>
-    <row r="47" spans="1:12" ht="15.75">
+        <f t="shared" ref="I46:I77" si="3">H46/$K$6*10*$K$5</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="75"/>
+      <c r="K46" s="74"/>
+      <c r="L46" s="74"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.75">
       <c r="A47" s="52" t="s">
         <v>122</v>
       </c>
@@ -4806,21 +4995,25 @@
         <v>5</v>
       </c>
       <c r="I47" s="49">
+        <f t="shared" si="3"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="J47" s="116">
+        <v>1</v>
+      </c>
+      <c r="K47" s="117">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="L47" s="117">
         <f t="shared" si="2"/>
-        <v>0.41666666666666663</v>
-      </c>
-      <c r="J47" s="104">
-        <v>0.1</v>
-      </c>
-      <c r="K47" s="103">
-        <f t="shared" si="1"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L47" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="M47" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75">
+    <row r="48" spans="1:14" ht="15.75">
       <c r="A48" s="44" t="s">
         <v>120</v>
       </c>
@@ -4844,21 +5037,28 @@
         <v>8</v>
       </c>
       <c r="I48" s="39">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J48" s="116">
+        <v>0.5</v>
+      </c>
+      <c r="K48" s="117">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L48" s="117">
         <f t="shared" si="2"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J48" s="104">
-        <v>0.1</v>
-      </c>
-      <c r="K48" s="103">
-        <f t="shared" si="1"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="L48" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M48" s="118" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" ht="15.75">
+      <c r="N48" s="23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="15.75">
       <c r="A49" s="44" t="s">
         <v>119</v>
       </c>
@@ -4882,21 +5082,28 @@
         <v>7</v>
       </c>
       <c r="I49" s="39">
+        <f t="shared" si="3"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="J49" s="116">
+        <v>0</v>
+      </c>
+      <c r="K49" s="117">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L49" s="117">
         <f t="shared" si="2"/>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="J49" s="104">
-        <v>0.1</v>
-      </c>
-      <c r="K49" s="103">
-        <f t="shared" si="1"/>
-        <v>5.8333333333333341E-2</v>
-      </c>
-      <c r="L49" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="M49" s="118" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" ht="15.75">
+      <c r="N49" s="23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="15.75">
       <c r="A50" s="44" t="s">
         <v>117</v>
       </c>
@@ -4920,24 +5127,28 @@
         <v>7</v>
       </c>
       <c r="I50" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="J50" s="104">
+      <c r="J50" s="116">
         <v>0.8</v>
       </c>
-      <c r="K50" s="103">
+      <c r="K50" s="117">
         <f t="shared" si="1"/>
         <v>0.46666666666666673</v>
       </c>
-      <c r="L50" s="23" t="s">
+      <c r="L50" s="117">
+        <f t="shared" si="2"/>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="M50" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="M50" s="23" t="s">
+      <c r="N50" s="23" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="15.75">
+    <row r="51" spans="1:14" ht="15.75">
       <c r="A51" s="44" t="s">
         <v>115</v>
       </c>
@@ -4961,24 +5172,28 @@
         <v>10</v>
       </c>
       <c r="I51" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.83333333333333326</v>
       </c>
-      <c r="J51" s="104">
+      <c r="J51" s="116">
         <v>0.1</v>
       </c>
-      <c r="K51" s="103">
+      <c r="K51" s="117">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="L51" s="23" t="s">
+      <c r="L51" s="117">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M51" s="118" t="s">
         <v>222</v>
       </c>
-      <c r="M51" s="23" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="15.75">
+      <c r="N51" s="23" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="15.75">
       <c r="A52" s="44" t="s">
         <v>112</v>
       </c>
@@ -5002,21 +5217,25 @@
         <v>10</v>
       </c>
       <c r="I52" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.83333333333333326</v>
       </c>
-      <c r="J52" s="104">
+      <c r="J52" s="116">
         <v>0.9</v>
       </c>
-      <c r="K52" s="103">
+      <c r="K52" s="117">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L52" s="23" t="s">
+      <c r="L52" s="117">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M52" s="118" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="15.75">
+    <row r="53" spans="1:14" ht="15.75">
       <c r="A53" s="44" t="s">
         <v>111</v>
       </c>
@@ -5040,21 +5259,25 @@
         <v>13</v>
       </c>
       <c r="I53" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0833333333333335</v>
       </c>
-      <c r="J53" s="104">
+      <c r="J53" s="116">
         <v>1</v>
       </c>
-      <c r="K53" s="103">
+      <c r="K53" s="117">
         <f t="shared" si="1"/>
         <v>1.0833333333333335</v>
       </c>
-      <c r="L53" s="23" t="s">
+      <c r="L53" s="117">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="M53" s="118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="15.75">
+    <row r="54" spans="1:14" ht="15.75">
       <c r="A54" s="44" t="s">
         <v>109</v>
       </c>
@@ -5078,21 +5301,25 @@
         <v>9</v>
       </c>
       <c r="I54" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="J54" s="104">
+      <c r="J54" s="116">
         <v>1</v>
       </c>
-      <c r="K54" s="103">
+      <c r="K54" s="117">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L54" s="23" t="s">
+      <c r="L54" s="117">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M54" s="118" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15.75">
+    <row r="55" spans="1:14" ht="15.75">
       <c r="A55" s="44" t="s">
         <v>107</v>
       </c>
@@ -5116,24 +5343,28 @@
         <v>9</v>
       </c>
       <c r="I55" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="J55" s="104">
+      <c r="J55" s="116">
         <v>0.9</v>
       </c>
-      <c r="K55" s="103">
+      <c r="K55" s="117">
         <f t="shared" si="1"/>
         <v>0.67500000000000004</v>
       </c>
-      <c r="L55" s="23" t="s">
+      <c r="L55" s="117">
+        <f t="shared" si="2"/>
+        <v>8.1</v>
+      </c>
+      <c r="M55" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="M55" s="23" t="s">
+      <c r="N55" s="23" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.75">
+    <row r="56" spans="1:14" ht="15.75">
       <c r="A56" s="44" t="s">
         <v>105</v>
       </c>
@@ -5157,21 +5388,25 @@
         <v>9</v>
       </c>
       <c r="I56" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="J56" s="104">
+      <c r="J56" s="116">
         <v>1</v>
       </c>
-      <c r="K56" s="103">
+      <c r="K56" s="117">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L56" s="23" t="s">
+      <c r="L56" s="117">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M56" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="15.75">
+    <row r="57" spans="1:14" ht="15.75">
       <c r="A57" s="44" t="s">
         <v>103</v>
       </c>
@@ -5195,21 +5430,25 @@
         <v>9</v>
       </c>
       <c r="I57" s="39">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="J57" s="116">
+        <v>0</v>
+      </c>
+      <c r="K57" s="117">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L57" s="117">
         <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
-      <c r="J57" s="104">
-        <v>0</v>
-      </c>
-      <c r="K57" s="103">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L57" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="M57" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="15.75">
+    <row r="58" spans="1:14" ht="15.75">
       <c r="A58" s="44" t="s">
         <v>100</v>
       </c>
@@ -5233,24 +5472,28 @@
         <v>8</v>
       </c>
       <c r="I58" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J58" s="104">
+      <c r="J58" s="116">
         <v>0.5</v>
       </c>
-      <c r="K58" s="103">
+      <c r="K58" s="117">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="L58" s="23" t="s">
+      <c r="L58" s="117">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="M58" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="M58" s="23" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="15.75">
+      <c r="N58" s="23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="15.75">
       <c r="A59" s="44" t="s">
         <v>98</v>
       </c>
@@ -5272,13 +5515,14 @@
       </c>
       <c r="H59" s="40"/>
       <c r="I59" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J59" s="104"/>
-      <c r="K59" s="103"/>
-    </row>
-    <row r="60" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="75"/>
+      <c r="K59" s="74"/>
+      <c r="L59" s="74"/>
+    </row>
+    <row r="60" spans="1:14" ht="15.75">
       <c r="A60" s="44" t="s">
         <v>96</v>
       </c>
@@ -5300,13 +5544,14 @@
       </c>
       <c r="H60" s="40"/>
       <c r="I60" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J60" s="104"/>
-      <c r="K60" s="103"/>
-    </row>
-    <row r="61" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J60" s="75"/>
+      <c r="K60" s="74"/>
+      <c r="L60" s="74"/>
+    </row>
+    <row r="61" spans="1:14" ht="15.75">
       <c r="A61" s="44" t="s">
         <v>94</v>
       </c>
@@ -5328,13 +5573,14 @@
       </c>
       <c r="H61" s="40"/>
       <c r="I61" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J61" s="104"/>
-      <c r="K61" s="103"/>
-    </row>
-    <row r="62" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J61" s="75"/>
+      <c r="K61" s="74"/>
+      <c r="L61" s="74"/>
+    </row>
+    <row r="62" spans="1:14" ht="15.75">
       <c r="A62" s="44" t="s">
         <v>93</v>
       </c>
@@ -5356,13 +5602,14 @@
       </c>
       <c r="H62" s="40"/>
       <c r="I62" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J62" s="104"/>
-      <c r="K62" s="103"/>
-    </row>
-    <row r="63" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J62" s="75"/>
+      <c r="K62" s="74"/>
+      <c r="L62" s="74"/>
+    </row>
+    <row r="63" spans="1:14" ht="15.75">
       <c r="A63" s="44" t="s">
         <v>89</v>
       </c>
@@ -5386,24 +5633,28 @@
         <v>33</v>
       </c>
       <c r="I63" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.75</v>
       </c>
-      <c r="J63" s="104">
+      <c r="J63" s="116">
         <v>0.1</v>
       </c>
-      <c r="K63" s="103">
+      <c r="K63" s="117">
         <f t="shared" si="1"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="L63" s="23" t="s">
+      <c r="L63" s="117">
+        <f t="shared" si="2"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="M63" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="M63" s="23" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="15.75">
+      <c r="N63" s="23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="15.75">
       <c r="A64" s="44" t="s">
         <v>87</v>
       </c>
@@ -5425,13 +5676,14 @@
       </c>
       <c r="H64" s="40"/>
       <c r="I64" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J64" s="104"/>
-      <c r="K64" s="103"/>
-    </row>
-    <row r="65" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J64" s="75"/>
+      <c r="K64" s="74"/>
+      <c r="L64" s="74"/>
+    </row>
+    <row r="65" spans="1:14" ht="15.75">
       <c r="A65" s="44" t="s">
         <v>85</v>
       </c>
@@ -5455,24 +5707,28 @@
         <v>18</v>
       </c>
       <c r="I65" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="J65" s="104">
+      <c r="J65" s="116">
         <v>0.5</v>
       </c>
-      <c r="K65" s="103">
+      <c r="K65" s="117">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L65" s="23" t="s">
+      <c r="L65" s="117">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M65" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="M65" s="23" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="15.75">
+      <c r="N65" s="23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="15.75">
       <c r="A66" s="44" t="s">
         <v>83</v>
       </c>
@@ -5494,13 +5750,14 @@
       </c>
       <c r="H66" s="40"/>
       <c r="I66" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J66" s="104"/>
-      <c r="K66" s="103"/>
-    </row>
-    <row r="67" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J66" s="75"/>
+      <c r="K66" s="74"/>
+      <c r="L66" s="74"/>
+    </row>
+    <row r="67" spans="1:14" ht="15.75">
       <c r="A67" s="44" t="s">
         <v>81</v>
       </c>
@@ -5522,13 +5779,14 @@
       </c>
       <c r="H67" s="40"/>
       <c r="I67" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J67" s="104"/>
-      <c r="K67" s="103"/>
-    </row>
-    <row r="68" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J67" s="75"/>
+      <c r="K67" s="74"/>
+      <c r="L67" s="74"/>
+    </row>
+    <row r="68" spans="1:14" ht="15.75">
       <c r="A68" s="44" t="s">
         <v>79</v>
       </c>
@@ -5550,13 +5808,14 @@
       </c>
       <c r="H68" s="40"/>
       <c r="I68" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J68" s="104"/>
-      <c r="K68" s="103"/>
-    </row>
-    <row r="69" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J68" s="75"/>
+      <c r="K68" s="74"/>
+      <c r="L68" s="74"/>
+    </row>
+    <row r="69" spans="1:14" ht="15.75">
       <c r="A69" s="44" t="s">
         <v>77</v>
       </c>
@@ -5578,13 +5837,14 @@
       </c>
       <c r="H69" s="40"/>
       <c r="I69" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J69" s="104"/>
-      <c r="K69" s="103"/>
-    </row>
-    <row r="70" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J69" s="75"/>
+      <c r="K69" s="74"/>
+      <c r="L69" s="74"/>
+    </row>
+    <row r="70" spans="1:14" ht="15.75">
       <c r="A70" s="44" t="s">
         <v>75</v>
       </c>
@@ -5606,13 +5866,14 @@
       </c>
       <c r="H70" s="40"/>
       <c r="I70" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J70" s="104"/>
-      <c r="K70" s="103"/>
-    </row>
-    <row r="71" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J70" s="75"/>
+      <c r="K70" s="74"/>
+      <c r="L70" s="74"/>
+    </row>
+    <row r="71" spans="1:14" ht="15.75">
       <c r="A71" s="44" t="s">
         <v>72</v>
       </c>
@@ -5634,13 +5895,14 @@
       </c>
       <c r="H71" s="40"/>
       <c r="I71" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J71" s="104"/>
-      <c r="K71" s="103"/>
-    </row>
-    <row r="72" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J71" s="75"/>
+      <c r="K71" s="74"/>
+      <c r="L71" s="74"/>
+    </row>
+    <row r="72" spans="1:14" ht="15.75">
       <c r="A72" s="44" t="s">
         <v>70</v>
       </c>
@@ -5662,13 +5924,14 @@
       </c>
       <c r="H72" s="40"/>
       <c r="I72" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J72" s="104"/>
-      <c r="K72" s="103"/>
-    </row>
-    <row r="73" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J72" s="75"/>
+      <c r="K72" s="74"/>
+      <c r="L72" s="74"/>
+    </row>
+    <row r="73" spans="1:14" ht="15.75">
       <c r="A73" s="44" t="s">
         <v>68</v>
       </c>
@@ -5690,13 +5953,14 @@
       </c>
       <c r="H73" s="40"/>
       <c r="I73" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J73" s="104"/>
-      <c r="K73" s="103"/>
-    </row>
-    <row r="74" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J73" s="75"/>
+      <c r="K73" s="74"/>
+      <c r="L73" s="74"/>
+    </row>
+    <row r="74" spans="1:14" ht="15.75">
       <c r="A74" s="44" t="s">
         <v>65</v>
       </c>
@@ -5718,13 +5982,14 @@
       </c>
       <c r="H74" s="40"/>
       <c r="I74" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J74" s="104"/>
-      <c r="K74" s="103"/>
-    </row>
-    <row r="75" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J74" s="75"/>
+      <c r="K74" s="74"/>
+      <c r="L74" s="74"/>
+    </row>
+    <row r="75" spans="1:14" ht="15.75">
       <c r="A75" s="44" t="s">
         <v>63</v>
       </c>
@@ -5746,13 +6011,14 @@
       </c>
       <c r="H75" s="40"/>
       <c r="I75" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J75" s="104"/>
-      <c r="K75" s="103"/>
-    </row>
-    <row r="76" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J75" s="75"/>
+      <c r="K75" s="74"/>
+      <c r="L75" s="74"/>
+    </row>
+    <row r="76" spans="1:14" ht="15.75">
       <c r="A76" s="44" t="s">
         <v>61</v>
       </c>
@@ -5774,13 +6040,14 @@
       </c>
       <c r="H76" s="40"/>
       <c r="I76" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J76" s="104"/>
-      <c r="K76" s="103"/>
-    </row>
-    <row r="77" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J76" s="75"/>
+      <c r="K76" s="74"/>
+      <c r="L76" s="74"/>
+    </row>
+    <row r="77" spans="1:14" ht="15.75">
       <c r="A77" s="44" t="s">
         <v>60</v>
       </c>
@@ -5802,13 +6069,14 @@
       </c>
       <c r="H77" s="40"/>
       <c r="I77" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J77" s="104"/>
-      <c r="K77" s="103"/>
-    </row>
-    <row r="78" spans="1:13" ht="15.75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J77" s="75"/>
+      <c r="K77" s="74"/>
+      <c r="L77" s="74"/>
+    </row>
+    <row r="78" spans="1:14" ht="15.75">
       <c r="A78" s="44" t="s">
         <v>58</v>
       </c>
@@ -5833,10 +6101,11 @@
         <f>H78/$K$6*10*$K$5</f>
         <v>0</v>
       </c>
-      <c r="J78" s="104"/>
-      <c r="K78" s="103"/>
-    </row>
-    <row r="79" spans="1:13" ht="15.75">
+      <c r="J78" s="75"/>
+      <c r="K78" s="74"/>
+      <c r="L78" s="74"/>
+    </row>
+    <row r="79" spans="1:14" ht="15.75">
       <c r="A79" s="44" t="s">
         <v>54</v>
       </c>
@@ -5863,18 +6132,22 @@
         <f>H79/$K$6*10*$K$5</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="J79" s="104">
+      <c r="J79" s="116">
         <v>1</v>
       </c>
-      <c r="K79" s="103">
+      <c r="K79" s="117">
         <f>I79*J79</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="L79" s="23" t="s">
+      <c r="L79" s="117">
+        <f t="shared" ref="L79:L82" si="4">H79*J79</f>
+        <v>7</v>
+      </c>
+      <c r="M79" s="118" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="15.75">
+    <row r="80" spans="1:14" ht="15.75">
       <c r="A80" s="44" t="s">
         <v>53</v>
       </c>
@@ -5899,10 +6172,11 @@
         <f>H80/$K$6*10*$K$5</f>
         <v>0</v>
       </c>
-      <c r="J80" s="104"/>
-      <c r="K80" s="103"/>
-    </row>
-    <row r="81" spans="1:11" ht="15.75">
+      <c r="J80" s="75"/>
+      <c r="K80" s="74"/>
+      <c r="L80" s="74"/>
+    </row>
+    <row r="81" spans="1:12" ht="15.75">
       <c r="A81" s="44" t="s">
         <v>52</v>
       </c>
@@ -5927,10 +6201,11 @@
         <f>H81/$K$6*10*$K$5</f>
         <v>0</v>
       </c>
-      <c r="J81" s="104"/>
-      <c r="K81" s="103"/>
-    </row>
-    <row r="82" spans="1:11" ht="15.75">
+      <c r="J81" s="75"/>
+      <c r="K81" s="74"/>
+      <c r="L81" s="74"/>
+    </row>
+    <row r="82" spans="1:12" ht="15.75">
       <c r="A82" s="44" t="s">
         <v>51</v>
       </c>
@@ -5955,36 +6230,58 @@
         <f>H82/$K$6*10*$K$5</f>
         <v>0</v>
       </c>
-      <c r="J82" s="104"/>
-      <c r="K82" s="103"/>
-    </row>
-    <row r="83" spans="1:11">
-      <c r="J83" s="23" t="s">
+      <c r="J82" s="75"/>
+      <c r="K82" s="74"/>
+      <c r="L82" s="74"/>
+    </row>
+    <row r="83" spans="1:12" ht="15.75" customHeight="1">
+      <c r="I83" s="119" t="s">
         <v>226</v>
       </c>
-      <c r="K83" s="23">
+      <c r="J83" s="119"/>
+      <c r="K83" s="118">
         <f>SUM(K14:K82)</f>
-        <v>19.739166666666666</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11">
-      <c r="J84" s="23" t="s">
+        <v>20.549999999999997</v>
+      </c>
+      <c r="L83" s="117">
+        <f>SUM(L14:L82)</f>
+        <v>246.6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="J84" s="120" t="s">
         <v>227</v>
       </c>
-      <c r="K84" s="23">
+      <c r="K84" s="117">
         <f>K83/K9*10</f>
-        <v>7.2883076923076926</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11">
-      <c r="J85" s="103"/>
-      <c r="K85" s="23">
+        <v>7.5876923076923077</v>
+      </c>
+      <c r="L84" s="118">
+        <f>L83/K6*10</f>
+        <v>10.275</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="J85" s="74"/>
+      <c r="K85" s="117">
         <f>2/3*K84</f>
-        <v>4.8588717948717948</v>
+        <v>5.0584615384615379</v>
+      </c>
+      <c r="L85" s="117">
+        <f>2/3*L84</f>
+        <v>6.85</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="E5:J5"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="E8:J8"/>
@@ -5995,14 +6292,8 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E4:K4"/>
-    <mergeCell ref="E5:J5"/>
   </mergeCells>
-  <conditionalFormatting sqref="K8">
+  <conditionalFormatting sqref="K8:L8">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>

</xml_diff>